<commit_message>
Se agrego el modulo para salir de SAP Se arreglo la logica para agregar los errores al excel
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Documents\UiPath\Proceso1_LALA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4130EC19-2B93-48E8-AC92-AB4A7EE223ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3C3BFE-196E-4FBC-9037-5AD3F61435CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -157,9 +157,6 @@
     <t>email_To</t>
   </si>
   <si>
-    <t>donal_nar@hotmail.com</t>
-  </si>
-  <si>
     <t>cruzleonardo00@gmail.com</t>
   </si>
   <si>
@@ -170,13 +167,16 @@
   </si>
   <si>
     <t>donaldo.cruz@kirjner.edu.mx</t>
+  </si>
+  <si>
+    <t>donaldo.cruz@beeckerco.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -206,6 +206,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -228,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -239,6 +245,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -557,7 +564,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -675,18 +682,18 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1678,9 +1685,9 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{0DC83872-0326-4C9C-9FD2-5B7A39A9885C}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{B53E7484-0D43-44B3-9ED6-813990F665EF}"/>
-    <hyperlink ref="B11" r:id="rId3" xr:uid="{6C058642-9F03-49DC-9941-8449E2D0D7A9}"/>
-    <hyperlink ref="B12" r:id="rId4" xr:uid="{D425E0A2-8319-405C-A87D-4A91E2272181}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{6C058642-9F03-49DC-9941-8449E2D0D7A9}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{D425E0A2-8319-405C-A87D-4A91E2272181}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{2F329549-AB91-4377-8DB9-2172E448D55C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>